<commit_message>
add pillars scene kpis
</commit_message>
<xml_diff>
--- a/Projects/CCUS/Pillars/Data/Template.xlsx
+++ b/Projects/CCUS/Pillars/Data/Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Programs" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">Program Name</t>
   </si>
@@ -28,16 +28,16 @@
     <t xml:space="preserve">brand_name</t>
   </si>
   <si>
+    <t xml:space="preserve">display_brand_name</t>
+  </si>
+  <si>
     <t xml:space="preserve">quri_name</t>
   </si>
   <si>
-    <t xml:space="preserve">display_id</t>
-  </si>
-  <si>
     <t xml:space="preserve">survey_question</t>
   </si>
   <si>
-    <t xml:space="preserve">Survey Target_answer</t>
+    <t xml:space="preserve">survey_target_answer</t>
   </si>
   <si>
     <t xml:space="preserve">start_date</t>
@@ -62,6 +62,24 @@
   </si>
   <si>
     <t xml:space="preserve">Warm Display with NCAA March Madness POS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warm Display with Hydration POS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Big Games</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warm Display with Big Game POS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spring/ Summer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warm Display with Spring/Summer POS</t>
   </si>
 </sst>
 </file>
@@ -72,7 +90,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -93,6 +111,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <u val="single"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,17 +163,29 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -167,77 +205,123 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="7.96428571428571"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="2" t="n">
-        <v>43466</v>
-      </c>
-      <c r="H2" s="2" t="n">
-        <v>43831</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="G2" s="5" t="n">
+        <v>43466</v>
+      </c>
+      <c r="H2" s="5" t="n">
+        <v>43831</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="2" t="n">
-        <v>43466</v>
-      </c>
-      <c r="H3" s="2" t="n">
+      <c r="G3" s="5" t="n">
+        <v>43466</v>
+      </c>
+      <c r="H3" s="5" t="n">
+        <v>43831</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>43466</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>43831</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>43466</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <v>43831</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>43466</v>
+      </c>
+      <c r="H6" s="5" t="n">
         <v>43831</v>
       </c>
     </row>

</xml_diff>